<commit_message>
Added Graphs to Report, missing Connectivity part
</commit_message>
<xml_diff>
--- a/Entrega_II/DFSandBFSComparison.xlsx
+++ b/Entrega_II/DFSandBFSComparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GoncaloAlves\Desktop\FEUP\2_Ano\MeatWagons\Entrega_II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E34A101F-F9A6-4C1B-9E14-A49ADE0E3A26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{99B727A0-DC17-49EC-9F96-4FEF71460602}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -587,6 +587,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Comparação DFS e BFS</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -627,7 +652,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>DFSandBFSComparison!$B$1</c:f>
+              <c:f>DFSandBFSComparison!$B$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -660,171 +685,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-1.1745404335906742E-3"/>
-                  <c:y val="-0.23316981343535201"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-FC30-4386-BDBE-05918DC01062}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="4.1446187065444576E-2"/>
-                  <c:y val="-0.2448649844853967"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000004-FC30-4386-BDBE-05918DC01062}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="8.6513920272672726E-2"/>
-                  <c:y val="-0.24861299351587418"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000003-FC30-4386-BDBE-05918DC01062}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="2.8329054233408582E-3"/>
-                  <c:y val="-2.1711896618699864E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000A-FC30-4386-BDBE-05918DC01062}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-2.8329054233409102E-3"/>
-                  <c:y val="-6.9960555771365937E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000B-FC30-4386-BDBE-05918DC01062}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pt-PT"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>DFSandBFSComparison!$A$2:$A$7</c:f>
+              <c:f>DFSandBFSComparison!$A$10:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -851,27 +714,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>DFSandBFSComparison!$B$2:$B$7</c:f>
+              <c:f>DFSandBFSComparison!$B$10:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>185</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>188</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>189</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1118</c:v>
+                  <c:v>1417</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>475</c:v>
+                  <c:v>2461</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5991</c:v>
+                  <c:v>7886</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -879,7 +742,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FC30-4386-BDBE-05918DC01062}"/>
+              <c16:uniqueId val="{00000000-2E93-41DB-8DB5-E4C001B2EAB7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -888,7 +751,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>DFSandBFSComparison!$C$1</c:f>
+              <c:f>DFSandBFSComparison!$C$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -921,171 +784,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="0"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-1.4164527116704551E-3"/>
-                  <c:y val="-0.20023193548356449"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000009-FC30-4386-BDBE-05918DC01062}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="1"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="3.9660675926772714E-2"/>
-                  <c:y val="-0.19540706956829806"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000008-FC30-4386-BDBE-05918DC01062}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="8.6403615411897755E-2"/>
-                  <c:y val="-0.2050568013988312"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000007-FC30-4386-BDBE-05918DC01062}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="1.4164527116704031E-3"/>
-                  <c:y val="4.3423793237399373E-2"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000006-FC30-4386-BDBE-05918DC01062}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="4"/>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="2.8329054233409102E-3"/>
-                  <c:y val="4.8248659152666162E-3"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{0000000C-FC30-4386-BDBE-05918DC01062}"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="pt-PT"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>DFSandBFSComparison!$A$2:$A$7</c:f>
+              <c:f>DFSandBFSComparison!$A$10:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1112,27 +813,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>DFSandBFSComparison!$C$2:$C$7</c:f>
+              <c:f>DFSandBFSComparison!$C$10:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>183</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>192</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>189</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>707</c:v>
+                  <c:v>691</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>209</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4256</c:v>
+                  <c:v>3676</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1140,7 +841,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FC30-4386-BDBE-05918DC01062}"/>
+              <c16:uniqueId val="{00000001-2E93-41DB-8DB5-E4C001B2EAB7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1152,13 +853,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1480684127"/>
-        <c:axId val="1571112575"/>
+        <c:axId val="1466348080"/>
+        <c:axId val="1462055600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1480684127"/>
+        <c:axId val="1466348080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="55000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1197,11 +900,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pt-PT"/>
-                  <a:t>Tamanho</a:t>
+                  <a:t>Tamanho do</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="pt-PT" baseline="0"/>
-                  <a:t> do Grafo</a:t>
+                  <a:t> Grafo (Número de vértices)</a:t>
                 </a:r>
                 <a:endParaRPr lang="pt-PT"/>
               </a:p>
@@ -1273,14 +976,15 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1571112575"/>
+        <c:crossAx val="1462055600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1571112575"/>
+        <c:axId val="1462055600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="8000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1318,7 +1022,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="pt-PT"/>
                   <a:t>Tempo de execução (</a:t>
                 </a:r>
                 <a:r>
@@ -1336,7 +1040,7 @@
                   <a:t>s</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="pt-PT"/>
                   <a:t>)</a:t>
                 </a:r>
               </a:p>
@@ -1408,7 +1112,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1480684127"/>
+        <c:crossAx val="1466348080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2049,22 +1753,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>7327</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>168519</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D742A32-303E-4570-AD33-56D0E9E407AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CD472F4-79CE-41BE-BB98-1953072140A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2382,89 +2086,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A9:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>25</v>
       </c>
-      <c r="B2">
-        <v>185</v>
+      <c r="B10">
+        <v>14</v>
       </c>
-      <c r="C2">
-        <v>183</v>
+      <c r="C10">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>81</v>
       </c>
-      <c r="B3">
-        <v>188</v>
+      <c r="B11">
+        <v>18</v>
       </c>
-      <c r="C3">
-        <v>192</v>
+      <c r="C11">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>289</v>
       </c>
-      <c r="B4">
-        <v>189</v>
+      <c r="B12">
+        <v>42</v>
       </c>
-      <c r="C4">
-        <v>189</v>
+      <c r="C12">
+        <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>10365</v>
       </c>
-      <c r="B5">
-        <v>1118</v>
+      <c r="B13">
+        <v>1417</v>
       </c>
-      <c r="C5">
-        <v>707</v>
+      <c r="C13">
+        <v>691</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>17772</v>
       </c>
-      <c r="B6">
-        <v>475</v>
+      <c r="B14">
+        <v>2461</v>
       </c>
-      <c r="C6">
-        <v>209</v>
+      <c r="C14">
+        <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>53621</v>
       </c>
-      <c r="B7">
-        <v>5991</v>
+      <c r="B15">
+        <v>7886</v>
       </c>
-      <c r="C7">
-        <v>4256</v>
+      <c r="C15">
+        <v>3676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>